<commit_message>
Updating some typos in assessment README
</commit_message>
<xml_diff>
--- a/data/sample_data.xlsx
+++ b/data/sample_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -79,16 +79,31 @@
     <t xml:space="preserve">Balance</t>
   </si>
   <si>
+    <t xml:space="preserve">Salaries:</t>
+  </si>
+  <si>
     <t xml:space="preserve">cash box</t>
   </si>
   <si>
     <t xml:space="preserve">salaries</t>
   </si>
   <si>
+    <t xml:space="preserve">Taxes:</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cash short</t>
   </si>
   <si>
+    <t xml:space="preserve">SS: </t>
+  </si>
+  <si>
     <t xml:space="preserve">cash balance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cashbox:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cash short:</t>
   </si>
   <si>
     <t xml:space="preserve">tax</t>
@@ -296,7 +311,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -737,8 +752,15 @@
         <f aca="false">D10-C10</f>
         <v>0</v>
       </c>
+      <c r="G10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <f aca="false">O7</f>
+        <v>141790</v>
+      </c>
       <c r="N10" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O10" s="3" t="n">
         <v>200000</v>
@@ -746,14 +768,21 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" s="2" t="n">
         <f aca="false">C7</f>
         <v>154000</v>
       </c>
+      <c r="G11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <f aca="false">N7</f>
+        <v>13450</v>
+      </c>
       <c r="N11" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="O11" s="3" t="n">
         <f aca="false">IF(O7&gt;O10, O7-O10, 0)</f>
@@ -769,8 +798,15 @@
         <v>8840</v>
       </c>
       <c r="D12" s="2"/>
+      <c r="G12" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <f aca="false">H7</f>
+        <v>13600</v>
+      </c>
       <c r="N12" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="O12" s="3" t="n">
         <f aca="false">O10-O7</f>
@@ -786,6 +822,13 @@
         <v>1400</v>
       </c>
       <c r="D13" s="2"/>
+      <c r="G13" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <f aca="false">O12</f>
+        <v>58210</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="4" t="s">
@@ -796,6 +839,13 @@
         <v>4600</v>
       </c>
       <c r="D14" s="2"/>
+      <c r="G14" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <f aca="false">O11</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="4" t="s">
@@ -809,7 +859,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D16" s="2" t="n">
         <f aca="false">N7</f>
@@ -818,7 +868,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D17" s="2" t="n">
         <f aca="false">O7</f>

</xml_diff>